<commit_message>
working on import issues
</commit_message>
<xml_diff>
--- a/data/demo_import_dataset.xlsx
+++ b/data/demo_import_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atana/Dev/electron/mil-tracker/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\group8\Documents\DEV\ai-e-nis\mil-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B990DAF9-2337-EF4B-A523-76E631173699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E01A072-6FC5-4628-BE16-85A7042BBDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" firstSheet="8" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="766" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,25 @@
     <sheet name="Equipment" sheetId="20" r:id="rId20"/>
     <sheet name="EquipmentAssignments" sheetId="21" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="224">
   <si>
     <t>name</t>
   </si>
@@ -706,6 +719,12 @@
   </si>
   <si>
     <t>COMMUNICATION</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>SP</t>
   </si>
 </sst>
 </file>
@@ -1073,9 +1092,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1119,9 +1138,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1129,7 +1148,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1137,7 +1156,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1156,9 +1175,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -1186,24 +1205,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1219,24 +1238,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -1250,15 +1269,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -1293,7 +1315,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -1304,7 +1326,7 @@
         <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -1316,7 +1338,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -1327,7 +1349,7 @@
         <v>117</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -1339,7 +1361,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -1350,7 +1372,7 @@
         <v>117</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -1362,7 +1384,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1373,7 +1395,7 @@
         <v>117</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -1385,7 +1407,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -1396,7 +1418,7 @@
         <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -1408,7 +1430,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -1419,7 +1441,7 @@
         <v>117</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -1431,7 +1453,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -1442,7 +1464,7 @@
         <v>117</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -1454,7 +1476,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -1465,7 +1487,7 @@
         <v>117</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -1477,7 +1499,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -1488,7 +1510,7 @@
         <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -1500,7 +1522,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -1511,7 +1533,7 @@
         <v>117</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -1523,7 +1545,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -1534,7 +1556,7 @@
         <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -1546,7 +1568,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -1557,7 +1579,7 @@
         <v>117</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -1569,7 +1591,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -1580,7 +1602,7 @@
         <v>117</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -1592,7 +1614,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -1603,7 +1625,7 @@
         <v>117</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -1615,7 +1637,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>145</v>
       </c>
@@ -1626,7 +1648,7 @@
         <v>117</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -1638,7 +1660,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>147</v>
       </c>
@@ -1649,7 +1671,7 @@
         <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
         <v>36</v>
@@ -1661,7 +1683,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -1672,7 +1694,7 @@
         <v>117</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
@@ -1684,7 +1706,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -1698,13 +1720,13 @@
         <v>154</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>155</v>
       </c>
@@ -1715,7 +1737,7 @@
         <v>117</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
         <v>44</v>
@@ -1724,7 +1746,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -1735,13 +1757,13 @@
         <v>117</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>222</v>
       </c>
       <c r="J21" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -1752,13 +1774,13 @@
         <v>117</v>
       </c>
       <c r="G22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>161</v>
       </c>
@@ -1769,13 +1791,13 @@
         <v>117</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>163</v>
       </c>
@@ -1786,13 +1808,13 @@
         <v>117</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>165</v>
       </c>
@@ -1803,13 +1825,13 @@
         <v>117</v>
       </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="J25" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>167</v>
       </c>
@@ -1820,7 +1842,7 @@
         <v>117</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J26" t="s">
         <v>118</v>
@@ -1837,9 +1859,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -1862,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -1882,7 +1904,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -1902,7 +1924,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -1933,9 +1955,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
@@ -1952,7 +1974,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -1969,7 +1991,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -1997,9 +2019,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
@@ -2013,7 +2035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -2024,7 +2046,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -2046,9 +2068,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
@@ -2071,7 +2093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -2091,7 +2113,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -2122,9 +2144,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -2165,7 +2187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -2197,7 +2219,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -2238,11 +2260,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2253,7 +2280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2264,7 +2291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2275,7 +2302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2286,7 +2313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2297,7 +2324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2308,7 +2335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2319,7 +2346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2330,7 +2357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2341,7 +2368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2352,7 +2379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2363,7 +2390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2374,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -2394,20 +2421,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2427,7 +2454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>201</v>
       </c>
@@ -2444,7 +2471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>204</v>
       </c>
@@ -2472,9 +2499,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>206</v>
       </c>
@@ -2494,7 +2521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>201</v>
       </c>
@@ -2514,7 +2541,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>204</v>
       </c>
@@ -2542,9 +2569,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2555,7 +2587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2566,7 +2598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2577,7 +2609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2588,7 +2620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2599,7 +2631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2623,9 +2655,9 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2642,7 +2674,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2659,7 +2691,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2676,7 +2708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -2693,7 +2725,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2710,7 +2742,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2727,7 +2759,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -2757,13 +2789,13 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2780,7 +2812,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2794,7 +2826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2821,16 +2853,16 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2859,7 +2891,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -2876,7 +2908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -2896,7 +2928,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -2913,7 +2945,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -2946,16 +2978,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2972,7 +3004,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -2989,7 +3021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -3000,7 +3032,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -3014,7 +3046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -3028,7 +3060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>218</v>
       </c>
@@ -3042,7 +3074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -3067,9 +3099,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
@@ -3092,7 +3124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3106,7 +3138,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -3131,9 +3163,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
@@ -3153,7 +3185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>

</xml_diff>